<commit_message>
fungsi generate jadwal fix, mau ke generate per mahasiswa
</commit_message>
<xml_diff>
--- a/myExcel.xlsx
+++ b/myExcel.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="43">
   <si>
     <t>ID Partikel</t>
   </si>
@@ -74,64 +74,73 @@
     <t>Deep Learning</t>
   </si>
   <si>
+    <t>Jumat</t>
+  </si>
+  <si>
+    <t>16:00 - 16:50</t>
+  </si>
+  <si>
+    <t>516</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>189</t>
+  </si>
+  <si>
+    <t>190</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>15:00 - 15:50</t>
+  </si>
+  <si>
+    <t>14:00 - 14:50</t>
+  </si>
+  <si>
+    <t>Rekayasa Perangkat Lunak Berbasis Komponen</t>
+  </si>
+  <si>
+    <t>11:00 - 11:50</t>
+  </si>
+  <si>
+    <t>08:00 - 08:50</t>
+  </si>
+  <si>
     <t>Kamis</t>
   </si>
   <si>
+    <t>Logika Informatika</t>
+  </si>
+  <si>
+    <t>09:00 - 09:50</t>
+  </si>
+  <si>
+    <t>191</t>
+  </si>
+  <si>
+    <t>192</t>
+  </si>
+  <si>
     <t>10:00 - 10:50</t>
   </si>
   <si>
-    <t>525</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>T</t>
-  </si>
-  <si>
-    <t>Jumat</t>
-  </si>
-  <si>
-    <t>Rekayasa Perangkat Lunak Berbasis Komponen</t>
-  </si>
-  <si>
-    <t>16:00 - 16:50</t>
-  </si>
-  <si>
-    <t>526</t>
-  </si>
-  <si>
-    <t>15:00 - 15:50</t>
-  </si>
-  <si>
-    <t>14:00 - 14:50</t>
-  </si>
-  <si>
-    <t>Pengembangan Rekayasa Perangkat Lunak Berbasis Service</t>
-  </si>
-  <si>
-    <t>11:00 - 11:50</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>09:00 - 09:50</t>
-  </si>
-  <si>
-    <t>08:00 - 08:50</t>
-  </si>
-  <si>
     <t>Etika Profesional</t>
   </si>
   <si>
     <t>6</t>
+  </si>
+  <si>
+    <t>13:00 - 13:50</t>
   </si>
 </sst>
 </file>
@@ -243,7 +252,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>138.0</v>
+        <v>249.0</v>
       </c>
       <c r="B2" t="s">
         <v>19</v>
@@ -278,12 +287,20 @@
       <c r="L2" t="s">
         <v>25</v>
       </c>
-      <c r="M2"/>
-      <c r="N2"/>
-      <c r="O2"/>
-      <c r="P2"/>
+      <c r="M2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P2" t="s">
+        <v>25</v>
+      </c>
       <c r="Q2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="R2" t="n">
         <v>1.0</v>
@@ -294,16 +311,16 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>139.0</v>
+        <v>250.0</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="E3" t="s">
         <v>22</v>
@@ -329,12 +346,20 @@
       <c r="L3" t="s">
         <v>25</v>
       </c>
-      <c r="M3"/>
-      <c r="N3"/>
-      <c r="O3"/>
-      <c r="P3"/>
+      <c r="M3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O3" t="s">
+        <v>25</v>
+      </c>
+      <c r="P3" t="s">
+        <v>25</v>
+      </c>
       <c r="Q3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="R3" t="n">
         <v>1.0</v>
@@ -345,47 +370,55 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>140.0</v>
+        <v>251.0</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" t="s">
+        <v>25</v>
+      </c>
+      <c r="L4" t="s">
+        <v>25</v>
+      </c>
+      <c r="M4" t="s">
+        <v>26</v>
+      </c>
+      <c r="N4" t="s">
         <v>27</v>
       </c>
-      <c r="D4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H4" t="s">
-        <v>25</v>
-      </c>
-      <c r="I4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J4" t="s">
-        <v>25</v>
-      </c>
-      <c r="K4" t="s">
-        <v>25</v>
-      </c>
-      <c r="L4" t="s">
-        <v>25</v>
-      </c>
-      <c r="M4"/>
-      <c r="N4"/>
-      <c r="O4"/>
-      <c r="P4"/>
+      <c r="O4" t="s">
+        <v>25</v>
+      </c>
+      <c r="P4" t="s">
+        <v>25</v>
+      </c>
       <c r="Q4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="R4" t="n">
         <v>1.0</v>
@@ -396,19 +429,19 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>141.0</v>
+        <v>252.0</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E5" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="F5" t="s">
         <v>24</v>
@@ -431,12 +464,20 @@
       <c r="L5" t="s">
         <v>25</v>
       </c>
-      <c r="M5"/>
-      <c r="N5"/>
-      <c r="O5"/>
-      <c r="P5"/>
+      <c r="M5" t="s">
+        <v>26</v>
+      </c>
+      <c r="N5" t="s">
+        <v>27</v>
+      </c>
+      <c r="O5" t="s">
+        <v>25</v>
+      </c>
+      <c r="P5" t="s">
+        <v>25</v>
+      </c>
       <c r="Q5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="R5" t="n">
         <v>1.0</v>
@@ -447,19 +488,19 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>142.0</v>
+        <v>253.0</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E6" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="F6" t="s">
         <v>24</v>
@@ -482,12 +523,20 @@
       <c r="L6" t="s">
         <v>25</v>
       </c>
-      <c r="M6"/>
-      <c r="N6"/>
-      <c r="O6"/>
-      <c r="P6"/>
+      <c r="M6" t="s">
+        <v>26</v>
+      </c>
+      <c r="N6" t="s">
+        <v>27</v>
+      </c>
+      <c r="O6" t="s">
+        <v>25</v>
+      </c>
+      <c r="P6" t="s">
+        <v>25</v>
+      </c>
       <c r="Q6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="R6" t="n">
         <v>1.0</v>
@@ -498,47 +547,55 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>143.0</v>
+        <v>254.0</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J7" t="s">
+        <v>25</v>
+      </c>
+      <c r="K7" t="s">
+        <v>25</v>
+      </c>
+      <c r="L7" t="s">
+        <v>25</v>
+      </c>
+      <c r="M7" t="s">
+        <v>26</v>
+      </c>
+      <c r="N7" t="s">
         <v>27</v>
       </c>
-      <c r="D7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" t="s">
-        <v>35</v>
-      </c>
-      <c r="G7" t="s">
-        <v>25</v>
-      </c>
-      <c r="H7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I7" t="s">
-        <v>25</v>
-      </c>
-      <c r="J7" t="s">
-        <v>25</v>
-      </c>
-      <c r="K7" t="s">
-        <v>25</v>
-      </c>
-      <c r="L7" t="s">
-        <v>25</v>
-      </c>
-      <c r="M7"/>
-      <c r="N7"/>
-      <c r="O7"/>
-      <c r="P7"/>
+      <c r="O7" t="s">
+        <v>25</v>
+      </c>
+      <c r="P7" t="s">
+        <v>25</v>
+      </c>
       <c r="Q7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="R7" t="n">
         <v>1.0</v>
@@ -549,10 +606,10 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>144.0</v>
+        <v>255.0</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C8" t="s">
         <v>20</v>
@@ -561,10 +618,10 @@
         <v>36</v>
       </c>
       <c r="E8" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="F8" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="G8" t="s">
         <v>25</v>
@@ -584,12 +641,20 @@
       <c r="L8" t="s">
         <v>25</v>
       </c>
-      <c r="M8"/>
-      <c r="N8"/>
-      <c r="O8"/>
-      <c r="P8"/>
+      <c r="M8" t="s">
+        <v>37</v>
+      </c>
+      <c r="N8" t="s">
+        <v>38</v>
+      </c>
+      <c r="O8" t="s">
+        <v>25</v>
+      </c>
+      <c r="P8" t="s">
+        <v>25</v>
+      </c>
       <c r="Q8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="R8" t="n">
         <v>1.0</v>
@@ -600,47 +665,55 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>145.0</v>
+        <v>256.0</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J9" t="s">
+        <v>25</v>
+      </c>
+      <c r="K9" t="s">
+        <v>25</v>
+      </c>
+      <c r="L9" t="s">
+        <v>25</v>
+      </c>
+      <c r="M9" t="s">
         <v>37</v>
       </c>
-      <c r="E9" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" t="s">
-        <v>35</v>
-      </c>
-      <c r="G9" t="s">
-        <v>25</v>
-      </c>
-      <c r="H9" t="s">
-        <v>25</v>
-      </c>
-      <c r="I9" t="s">
-        <v>25</v>
-      </c>
-      <c r="J9" t="s">
-        <v>25</v>
-      </c>
-      <c r="K9" t="s">
-        <v>25</v>
-      </c>
-      <c r="L9" t="s">
-        <v>25</v>
-      </c>
-      <c r="M9"/>
-      <c r="N9"/>
-      <c r="O9"/>
-      <c r="P9"/>
+      <c r="N9" t="s">
+        <v>38</v>
+      </c>
+      <c r="O9" t="s">
+        <v>25</v>
+      </c>
+      <c r="P9" t="s">
+        <v>25</v>
+      </c>
       <c r="Q9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="R9" t="n">
         <v>1.0</v>
@@ -651,22 +724,22 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>146.0</v>
+        <v>257.0</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="D10" t="s">
         <v>29</v>
       </c>
       <c r="E10" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="F10" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="G10" t="s">
         <v>25</v>
@@ -686,12 +759,20 @@
       <c r="L10" t="s">
         <v>25</v>
       </c>
-      <c r="M10"/>
-      <c r="N10"/>
-      <c r="O10"/>
-      <c r="P10"/>
+      <c r="M10" t="s">
+        <v>37</v>
+      </c>
+      <c r="N10" t="s">
+        <v>38</v>
+      </c>
+      <c r="O10" t="s">
+        <v>25</v>
+      </c>
+      <c r="P10" t="s">
+        <v>25</v>
+      </c>
       <c r="Q10" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="R10" t="n">
         <v>1.0</v>
@@ -702,47 +783,55 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>147.0</v>
+        <v>258.0</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" t="s">
+        <v>25</v>
+      </c>
+      <c r="I11" t="s">
+        <v>25</v>
+      </c>
+      <c r="J11" t="s">
+        <v>25</v>
+      </c>
+      <c r="K11" t="s">
+        <v>25</v>
+      </c>
+      <c r="L11" t="s">
+        <v>25</v>
+      </c>
+      <c r="M11" t="s">
+        <v>26</v>
+      </c>
+      <c r="N11" t="s">
         <v>27</v>
       </c>
-      <c r="D11" t="s">
-        <v>36</v>
-      </c>
-      <c r="E11" t="s">
-        <v>30</v>
-      </c>
-      <c r="F11" t="s">
-        <v>39</v>
-      </c>
-      <c r="G11" t="s">
-        <v>25</v>
-      </c>
-      <c r="H11" t="s">
-        <v>25</v>
-      </c>
-      <c r="I11" t="s">
-        <v>25</v>
-      </c>
-      <c r="J11" t="s">
-        <v>25</v>
-      </c>
-      <c r="K11" t="s">
-        <v>25</v>
-      </c>
-      <c r="L11" t="s">
-        <v>25</v>
-      </c>
-      <c r="M11"/>
-      <c r="N11"/>
-      <c r="O11"/>
-      <c r="P11"/>
+      <c r="O11" t="s">
+        <v>25</v>
+      </c>
+      <c r="P11" t="s">
+        <v>25</v>
+      </c>
       <c r="Q11" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="R11" t="n">
         <v>1.0</v>
@@ -753,22 +842,22 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>148.0</v>
+        <v>259.0</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="D12" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="E12" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="F12" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G12" t="s">
         <v>25</v>
@@ -788,12 +877,20 @@
       <c r="L12" t="s">
         <v>25</v>
       </c>
-      <c r="M12"/>
-      <c r="N12"/>
-      <c r="O12"/>
-      <c r="P12"/>
+      <c r="M12" t="s">
+        <v>26</v>
+      </c>
+      <c r="N12" t="s">
+        <v>27</v>
+      </c>
+      <c r="O12" t="s">
+        <v>25</v>
+      </c>
+      <c r="P12" t="s">
+        <v>25</v>
+      </c>
       <c r="Q12" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="R12" t="n">
         <v>1.0</v>

</xml_diff>